<commit_message>
creates + inserts update
</commit_message>
<xml_diff>
--- a/Sprint 3/USBD22/Dataset normalizado.xlsx
+++ b/Sprint 3/USBD22/Dataset normalizado.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Documentos\bddad2024\Sprint 3\USBD22\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandra\Desktop\BDDAD\bddad2024\Sprint 3\USBD22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B264FD31-7D9D-4FBA-9405-5D2A9207BBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C569BA-EEC6-475C-9C9E-F49FA80F93E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="700" activeTab="6" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="700" firstSheet="1" activeTab="6" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="246">
   <si>
     <t>Name</t>
   </si>
@@ -1381,7 +1381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8F968F-3FE6-476E-97DD-6EBBFE3BD57E}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -2917,7 +2917,7 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3730,7 +3730,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3926,7 +3926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C51F7F7-8394-4DF7-8369-AC46CFCEB4B5}">
   <dimension ref="A1:Q79"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
@@ -5012,10 +5012,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F07C3D1-0B8F-4AC3-A104-C9B8994DB4F3}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5263,28 +5263,12 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <v>12298</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="6">
-        <v>45108</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E11" s="5">
-        <v>10</v>
-      </c>
-      <c r="F11" s="5">
-        <v>10.25</v>
-      </c>
-      <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Procurement(SupplierId,ExternalPartId,StartDate,EndDate,MinQuantity,Price) VALUES(12298, 'AS12945G48', TO_DATE('01/07/2023', 'dd/MM/YYYY'), TO_DATE(NULL, 'dd/MM/YYYY'), 10, 10,25);</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -5302,84 +5286,33 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>12345</v>
+        <v>12298</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" ref="C15:C23" si="1">"INSERT INTO Supplier(" &amp; $A$13 &amp; ") VALUES(" &amp; A15 &amp; ");"</f>
-        <v>INSERT INTO Supplier(Id) VALUES(12345);</v>
+        <f>"INSERT INTO Supplier(" &amp; $A$13 &amp; ") VALUES(" &amp; A15 &amp; ");"</f>
+        <v>INSERT INTO Supplier(Id) VALUES(12298);</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <v>12345</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Supplier(Id) VALUES(12345);</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>12345</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Supplier(Id) VALUES(12345);</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <v>12345</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Supplier(Id) VALUES(12345);</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <v>12298</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Supplier(Id) VALUES(12298);</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
-        <v>12298</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Supplier(Id) VALUES(12298);</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>12298</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Supplier(Id) VALUES(12298);</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
-        <v>12298</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Supplier(Id) VALUES(12298);</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <v>12298</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO Supplier(Id) VALUES(12298);</v>
-      </c>
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6108,8 +6041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629B436D-7E6F-45CD-A274-6E2AE1A9129E}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7746,11 +7679,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7987,27 +7921,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE7026BE-4F45-4595-B98C-E9D8129D4591}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53C8F835-22B2-4A5C-B33C-2EBD4DAC13D0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c83fef03-7e53-47dc-8a06-28f89aa017e1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8032,9 +7956,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53C8F835-22B2-4A5C-B33C-2EBD4DAC13D0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE7026BE-4F45-4595-B98C-E9D8129D4591}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c83fef03-7e53-47dc-8a06-28f89aa017e1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>